<commit_message>
updated board game sheet Railroad Ink.
</commit_message>
<xml_diff>
--- a/info/桌游表格.xlsx
+++ b/info/桌游表格.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\felix\cc\boardGame\info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C22603C6-42DA-47E6-BD6E-541FB6309FFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{801FE601-EDD6-4926-B600-A0A35BEAD791}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14160" activeTab="6" xr2:uid="{454FEC03-9801-49D0-A78C-438D7E92AF31}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1640" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1640" uniqueCount="107">
   <si>
     <t>+</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -374,6 +374,9 @@
     <t/>
   </si>
   <si>
+    <t>round</t>
+  </si>
+  <si>
     <t>Railroad Ink:Deep Blue Edition(2018)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -438,6 +441,10 @@
     <t>____
 --
 ____</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>total</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -789,7 +796,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="152">
+  <borders count="153">
     <border>
       <left/>
       <right/>
@@ -2698,13 +2705,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="492">
+  <cellXfs count="510">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -4179,6 +4197,60 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="105" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="105" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="152" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -35766,7 +35838,7 @@
   <dimension ref="B1:AJ52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AO23" sqref="AO23"/>
+      <selection activeCell="AK17" sqref="AK17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -35777,7 +35849,7 @@
     <row r="1" spans="2:34" ht="14.5" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:34" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="425" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C2" s="426"/>
       <c r="D2" s="426"/>
@@ -35795,7 +35867,7 @@
       <c r="P2" s="426"/>
       <c r="Q2" s="427"/>
       <c r="S2" s="425" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="T2" s="426"/>
       <c r="U2" s="426"/>
@@ -35882,66 +35954,68 @@
       <c r="AH4" s="433"/>
     </row>
     <row r="5" spans="2:34" ht="14" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="434" t="s">
-        <v>91</v>
-      </c>
-      <c r="C5" s="435"/>
-      <c r="D5" s="435"/>
-      <c r="E5" s="436"/>
-      <c r="G5" s="434" t="s">
+      <c r="B5" s="497"/>
+      <c r="C5" s="499" t="s">
         <v>92</v>
       </c>
-      <c r="H5" s="435"/>
-      <c r="I5" s="436"/>
-      <c r="J5" s="437"/>
-      <c r="K5" s="434" t="s">
+      <c r="D5" s="440"/>
+      <c r="E5" s="440"/>
+      <c r="F5" s="440"/>
+      <c r="G5" s="441"/>
+      <c r="H5" s="499" t="s">
         <v>93</v>
       </c>
-      <c r="L5" s="436"/>
-      <c r="N5" s="438"/>
-      <c r="O5" s="439" t="s">
-        <v>94</v>
-      </c>
-      <c r="P5" s="440"/>
-      <c r="Q5" s="441"/>
+      <c r="I5" s="440"/>
+      <c r="J5" s="440"/>
+      <c r="K5" s="440"/>
+      <c r="L5" s="441"/>
+      <c r="M5" s="500" t="s">
+        <v>90</v>
+      </c>
+      <c r="N5" s="501"/>
+      <c r="O5" s="501"/>
+      <c r="P5" s="502"/>
+      <c r="Q5" s="492"/>
       <c r="S5" s="434" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="T5" s="435"/>
       <c r="U5" s="435"/>
       <c r="V5" s="436"/>
       <c r="X5" s="434" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="Y5" s="435"/>
       <c r="Z5" s="436"/>
       <c r="AA5" s="437"/>
       <c r="AB5" s="434" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AC5" s="436"/>
       <c r="AE5" s="438"/>
       <c r="AF5" s="439" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="AG5" s="440"/>
       <c r="AH5" s="441"/>
     </row>
     <row r="6" spans="2:34" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="442"/>
-      <c r="C6" s="443"/>
-      <c r="D6" s="443"/>
-      <c r="E6" s="444"/>
-      <c r="G6" s="442"/>
-      <c r="H6" s="443"/>
-      <c r="I6" s="444"/>
-      <c r="J6" s="437"/>
-      <c r="K6" s="442"/>
-      <c r="L6" s="444"/>
-      <c r="N6" s="437"/>
-      <c r="O6" s="434"/>
-      <c r="P6" s="435"/>
-      <c r="Q6" s="436"/>
+      <c r="B6" s="493"/>
+      <c r="C6" s="434"/>
+      <c r="D6" s="498"/>
+      <c r="E6" s="498"/>
+      <c r="F6" s="498"/>
+      <c r="G6" s="436"/>
+      <c r="H6" s="434"/>
+      <c r="I6" s="498"/>
+      <c r="J6" s="498"/>
+      <c r="K6" s="498"/>
+      <c r="L6" s="436"/>
+      <c r="M6" s="503"/>
+      <c r="N6" s="504"/>
+      <c r="O6" s="504"/>
+      <c r="P6" s="505"/>
+      <c r="Q6" s="494"/>
       <c r="S6" s="442"/>
       <c r="T6" s="443"/>
       <c r="U6" s="443"/>
@@ -35959,10 +36033,21 @@
     </row>
     <row r="7" spans="2:34" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="445"/>
-      <c r="N7" s="446"/>
-      <c r="O7" s="434"/>
-      <c r="P7" s="435"/>
-      <c r="Q7" s="436"/>
+      <c r="C7" s="442"/>
+      <c r="D7" s="443"/>
+      <c r="E7" s="443"/>
+      <c r="F7" s="443"/>
+      <c r="G7" s="444"/>
+      <c r="H7" s="442"/>
+      <c r="I7" s="443"/>
+      <c r="J7" s="443"/>
+      <c r="K7" s="443"/>
+      <c r="L7" s="444"/>
+      <c r="M7" s="506"/>
+      <c r="N7" s="507"/>
+      <c r="O7" s="507"/>
+      <c r="P7" s="508"/>
+      <c r="Q7" s="494"/>
       <c r="S7" s="445"/>
       <c r="AE7" s="446"/>
       <c r="AF7" s="434"/>
@@ -35972,77 +36057,79 @@
     <row r="8" spans="2:34" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="445"/>
       <c r="C8" s="447" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D8" s="448" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="449" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F8" s="448" t="s">
         <v>0</v>
       </c>
       <c r="G8" s="449" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H8" s="448" t="s">
         <v>0</v>
       </c>
       <c r="I8" s="449" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="J8" s="448" t="s">
         <v>0</v>
       </c>
       <c r="K8" s="449" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="L8" s="448" t="s">
         <v>0</v>
       </c>
       <c r="M8" s="450" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N8" s="451" t="s">
         <v>1</v>
       </c>
-      <c r="O8" s="442"/>
-      <c r="P8" s="443"/>
-      <c r="Q8" s="444"/>
+      <c r="O8" s="495" t="s">
+        <v>106</v>
+      </c>
+      <c r="P8" s="496"/>
+      <c r="Q8" s="509"/>
       <c r="S8" s="445"/>
       <c r="T8" s="447" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="U8" s="448" t="s">
         <v>0</v>
       </c>
       <c r="V8" s="449" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="W8" s="448" t="s">
         <v>0</v>
       </c>
       <c r="X8" s="449" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="Y8" s="448" t="s">
         <v>0</v>
       </c>
       <c r="Z8" s="449" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AA8" s="448" t="s">
         <v>0</v>
       </c>
       <c r="AB8" s="449" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AC8" s="448" t="s">
         <v>0</v>
       </c>
       <c r="AD8" s="450" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="AE8" s="451" t="s">
         <v>1</v>
@@ -36210,29 +36297,29 @@
     <row r="11" spans="2:34" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="445"/>
       <c r="E11" s="462" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F11" s="463"/>
       <c r="I11" s="464" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="J11" s="463"/>
       <c r="M11" s="462" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="N11" s="463"/>
       <c r="Q11" s="465"/>
       <c r="S11" s="445"/>
       <c r="V11" s="462" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="W11" s="463"/>
       <c r="Z11" s="464" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="AA11" s="463"/>
       <c r="AD11" s="462" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="AE11" s="463"/>
       <c r="AH11" s="465"/>
@@ -36307,7 +36394,7 @@
     </row>
     <row r="14" spans="2:34" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="471" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C14" s="468"/>
       <c r="D14" s="469"/>
@@ -36324,10 +36411,10 @@
       <c r="O14" s="469"/>
       <c r="P14" s="470"/>
       <c r="Q14" s="472" t="s">
+        <v>104</v>
+      </c>
+      <c r="S14" s="471" t="s">
         <v>103</v>
-      </c>
-      <c r="S14" s="471" t="s">
-        <v>102</v>
       </c>
       <c r="T14" s="468"/>
       <c r="U14" s="469"/>
@@ -36344,7 +36431,7 @@
       <c r="AF14" s="469"/>
       <c r="AG14" s="470"/>
       <c r="AH14" s="472" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="2:34" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -36451,7 +36538,7 @@
     </row>
     <row r="18" spans="2:36" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="483" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C18" s="468"/>
       <c r="D18" s="469"/>
@@ -36468,10 +36555,10 @@
       <c r="O18" s="469"/>
       <c r="P18" s="470"/>
       <c r="Q18" s="484" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="S18" s="483" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="T18" s="468"/>
       <c r="U18" s="469"/>
@@ -36488,7 +36575,7 @@
       <c r="AF18" s="469"/>
       <c r="AG18" s="470"/>
       <c r="AH18" s="484" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" spans="2:36" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -36595,7 +36682,7 @@
     </row>
     <row r="22" spans="2:36" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="471" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C22" s="468"/>
       <c r="D22" s="469"/>
@@ -36612,10 +36699,10 @@
       <c r="O22" s="469"/>
       <c r="P22" s="470"/>
       <c r="Q22" s="472" t="s">
+        <v>104</v>
+      </c>
+      <c r="S22" s="471" t="s">
         <v>103</v>
-      </c>
-      <c r="S22" s="471" t="s">
-        <v>102</v>
       </c>
       <c r="T22" s="468"/>
       <c r="U22" s="469"/>
@@ -36632,7 +36719,7 @@
       <c r="AF22" s="469"/>
       <c r="AG22" s="470"/>
       <c r="AH22" s="472" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="2:36" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -36743,19 +36830,19 @@
       <c r="C26" s="432"/>
       <c r="D26" s="432"/>
       <c r="E26" s="464" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F26" s="463"/>
       <c r="G26" s="432"/>
       <c r="H26" s="432"/>
       <c r="I26" s="462" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J26" s="463"/>
       <c r="K26" s="432"/>
       <c r="L26" s="432"/>
       <c r="M26" s="464" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="N26" s="463"/>
       <c r="O26" s="432"/>
@@ -36765,19 +36852,19 @@
       <c r="T26" s="432"/>
       <c r="U26" s="432"/>
       <c r="V26" s="464" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="W26" s="463"/>
       <c r="X26" s="432"/>
       <c r="Y26" s="432"/>
       <c r="Z26" s="462" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="AA26" s="463"/>
       <c r="AB26" s="432"/>
       <c r="AC26" s="432"/>
       <c r="AD26" s="464" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="AE26" s="463"/>
       <c r="AF26" s="432"/>
@@ -36787,7 +36874,7 @@
     <row r="27" spans="2:36" ht="14.5" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="28" spans="2:36" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B28" s="425" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C28" s="426"/>
       <c r="D28" s="426"/>
@@ -36805,7 +36892,7 @@
       <c r="P28" s="426"/>
       <c r="Q28" s="427"/>
       <c r="S28" s="425" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="T28" s="426"/>
       <c r="U28" s="426"/>
@@ -36893,46 +36980,46 @@
     </row>
     <row r="31" spans="2:36" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="434" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C31" s="435"/>
       <c r="D31" s="435"/>
       <c r="E31" s="436"/>
       <c r="G31" s="434" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H31" s="435"/>
       <c r="I31" s="436"/>
       <c r="J31" s="437"/>
       <c r="K31" s="434" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="L31" s="436"/>
       <c r="N31" s="438"/>
       <c r="O31" s="439" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="P31" s="440"/>
       <c r="Q31" s="441"/>
       <c r="S31" s="434" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="T31" s="435"/>
       <c r="U31" s="435"/>
       <c r="V31" s="436"/>
       <c r="X31" s="434" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="Y31" s="435"/>
       <c r="Z31" s="436"/>
       <c r="AA31" s="437"/>
       <c r="AB31" s="434" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AC31" s="436"/>
       <c r="AE31" s="438"/>
       <c r="AF31" s="439" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="AG31" s="440"/>
       <c r="AH31" s="441"/>
@@ -36982,37 +37069,37 @@
     <row r="34" spans="2:34" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B34" s="445"/>
       <c r="C34" s="447" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D34" s="448" t="s">
         <v>0</v>
       </c>
       <c r="E34" s="449" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F34" s="448" t="s">
         <v>0</v>
       </c>
       <c r="G34" s="449" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H34" s="448" t="s">
         <v>0</v>
       </c>
       <c r="I34" s="449" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="J34" s="448" t="s">
         <v>0</v>
       </c>
       <c r="K34" s="449" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="L34" s="448" t="s">
         <v>0</v>
       </c>
       <c r="M34" s="450" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N34" s="451" t="s">
         <v>1</v>
@@ -37022,37 +37109,37 @@
       <c r="Q34" s="444"/>
       <c r="S34" s="445"/>
       <c r="T34" s="447" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="U34" s="448" t="s">
         <v>0</v>
       </c>
       <c r="V34" s="449" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="W34" s="448" t="s">
         <v>0</v>
       </c>
       <c r="X34" s="449" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="Y34" s="448" t="s">
         <v>0</v>
       </c>
       <c r="Z34" s="449" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AA34" s="448" t="s">
         <v>0</v>
       </c>
       <c r="AB34" s="449" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AC34" s="448" t="s">
         <v>0</v>
       </c>
       <c r="AD34" s="450" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="AE34" s="451" t="s">
         <v>1</v>
@@ -37220,29 +37307,29 @@
     <row r="37" spans="2:34" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B37" s="445"/>
       <c r="E37" s="462" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F37" s="463"/>
       <c r="I37" s="464" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="J37" s="463"/>
       <c r="M37" s="462" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="N37" s="463"/>
       <c r="Q37" s="465"/>
       <c r="S37" s="445"/>
       <c r="V37" s="462" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="W37" s="463"/>
       <c r="Z37" s="464" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="AA37" s="463"/>
       <c r="AD37" s="462" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="AE37" s="463"/>
       <c r="AH37" s="465"/>
@@ -37317,7 +37404,7 @@
     </row>
     <row r="40" spans="2:34" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="471" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C40" s="468"/>
       <c r="D40" s="469"/>
@@ -37334,10 +37421,10 @@
       <c r="O40" s="469"/>
       <c r="P40" s="470"/>
       <c r="Q40" s="472" t="s">
+        <v>104</v>
+      </c>
+      <c r="S40" s="471" t="s">
         <v>103</v>
-      </c>
-      <c r="S40" s="471" t="s">
-        <v>102</v>
       </c>
       <c r="T40" s="468"/>
       <c r="U40" s="469"/>
@@ -37354,7 +37441,7 @@
       <c r="AF40" s="469"/>
       <c r="AG40" s="470"/>
       <c r="AH40" s="472" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="41" spans="2:34" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -37461,7 +37548,7 @@
     </row>
     <row r="44" spans="2:34" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44" s="483" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C44" s="468"/>
       <c r="D44" s="469"/>
@@ -37478,10 +37565,10 @@
       <c r="O44" s="469"/>
       <c r="P44" s="470"/>
       <c r="Q44" s="484" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="S44" s="483" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="T44" s="468"/>
       <c r="U44" s="469"/>
@@ -37498,7 +37585,7 @@
       <c r="AF44" s="469"/>
       <c r="AG44" s="470"/>
       <c r="AH44" s="484" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="45" spans="2:34" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -37605,7 +37692,7 @@
     </row>
     <row r="48" spans="2:34" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B48" s="471" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C48" s="468"/>
       <c r="D48" s="469"/>
@@ -37622,10 +37709,10 @@
       <c r="O48" s="469"/>
       <c r="P48" s="470"/>
       <c r="Q48" s="472" t="s">
+        <v>104</v>
+      </c>
+      <c r="S48" s="471" t="s">
         <v>103</v>
-      </c>
-      <c r="S48" s="471" t="s">
-        <v>102</v>
       </c>
       <c r="T48" s="468"/>
       <c r="U48" s="469"/>
@@ -37642,7 +37729,7 @@
       <c r="AF48" s="469"/>
       <c r="AG48" s="470"/>
       <c r="AH48" s="472" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="49" spans="2:34" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -37752,19 +37839,19 @@
       <c r="C52" s="432"/>
       <c r="D52" s="432"/>
       <c r="E52" s="464" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F52" s="463"/>
       <c r="G52" s="432"/>
       <c r="H52" s="432"/>
       <c r="I52" s="462" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J52" s="463"/>
       <c r="K52" s="432"/>
       <c r="L52" s="432"/>
       <c r="M52" s="464" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="N52" s="463"/>
       <c r="O52" s="432"/>
@@ -37774,19 +37861,19 @@
       <c r="T52" s="432"/>
       <c r="U52" s="432"/>
       <c r="V52" s="464" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="W52" s="463"/>
       <c r="X52" s="432"/>
       <c r="Y52" s="432"/>
       <c r="Z52" s="462" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="AA52" s="463"/>
       <c r="AB52" s="432"/>
       <c r="AC52" s="432"/>
       <c r="AD52" s="464" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="AE52" s="463"/>
       <c r="AF52" s="432"/>
@@ -37804,14 +37891,14 @@
     <mergeCell ref="AF9:AG9"/>
     <mergeCell ref="B2:Q2"/>
     <mergeCell ref="S2:AH2"/>
-    <mergeCell ref="B5:E6"/>
-    <mergeCell ref="G5:I6"/>
-    <mergeCell ref="K5:L6"/>
     <mergeCell ref="S5:V6"/>
     <mergeCell ref="X5:Z6"/>
     <mergeCell ref="AB5:AC6"/>
-    <mergeCell ref="O5:Q8"/>
     <mergeCell ref="AF5:AH8"/>
+    <mergeCell ref="C5:G7"/>
+    <mergeCell ref="H5:L7"/>
+    <mergeCell ref="M5:P7"/>
+    <mergeCell ref="O8:P8"/>
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="I11:J11"/>
     <mergeCell ref="M11:N11"/>
@@ -38086,6 +38173,7 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>